<commit_message>
nettoyage du code V2-7 et mise a jour des du fichier .xls (adresses)
</commit_message>
<xml_diff>
--- a/colombier.xlsx
+++ b/colombier.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ac81b492e88fac7c/Documents/_PROGRAMMES/_CUSTOMER/K_WASH/K-WASH_colombierP2/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\PROGRAMMES\_CUSTOMER\K_WASH\colombier\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A2EB2D1-73FB-4A7F-BA0A-E508BED456A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3DF1036-88AF-45EF-A690-04656D623379}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-24240" yWindow="1890" windowWidth="21600" windowHeight="13890" xr2:uid="{6FA983C0-EA7D-419E-8D78-023FE9FF8C70}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{6FA983C0-EA7D-419E-8D78-023FE9FF8C70}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="128">
   <si>
     <t>1-Q01</t>
   </si>
@@ -417,6 +417,9 @@
   </si>
   <si>
     <t>Amorcage pompes doseuses</t>
+  </si>
+  <si>
+    <t>Micro switch regul HP</t>
   </si>
 </sst>
 </file>
@@ -608,9 +611,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -648,7 +651,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -754,7 +757,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -896,7 +899,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -907,7 +910,7 @@
   <dimension ref="A2:G30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G23" sqref="G23"/>
+      <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1299,6 +1302,9 @@
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" s="9" t="s">
+        <v>127</v>
+      </c>
       <c r="B27" s="13" t="s">
         <v>117</v>
       </c>

</xml_diff>

<commit_message>
modif Q27 et Q29
</commit_message>
<xml_diff>
--- a/colombier.xlsx
+++ b/colombier.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\PROGRAMMES\_CUSTOMER\K_WASH\colombier\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3DF1036-88AF-45EF-A690-04656D623379}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9247CFDD-9704-43B6-9274-12F7455E4BFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{6FA983C0-EA7D-419E-8D78-023FE9FF8C70}"/>
+    <workbookView xWindow="-23610" yWindow="1110" windowWidth="16335" windowHeight="14505" xr2:uid="{6FA983C0-EA7D-419E-8D78-023FE9FF8C70}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -460,12 +460,24 @@
       <family val="3"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="9">
@@ -560,7 +572,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -593,6 +605,14 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -910,7 +930,7 @@
   <dimension ref="A2:G30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A27" sqref="A27"/>
+      <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -927,7 +947,7 @@
   <sheetData>
     <row r="2" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="9" t="s">
+      <c r="A3" s="16" t="s">
         <v>98</v>
       </c>
       <c r="B3" s="13" t="s">
@@ -945,12 +965,12 @@
       <c r="F3" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="G3" s="14" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="9" t="s">
+      <c r="A4" s="16" t="s">
         <v>99</v>
       </c>
       <c r="B4" s="13" t="s">
@@ -965,12 +985,12 @@
       <c r="F4" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="G4" s="1" t="s">
+      <c r="G4" s="14" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="9" t="s">
+      <c r="A5" s="16" t="s">
         <v>100</v>
       </c>
       <c r="B5" s="13" t="s">
@@ -985,12 +1005,12 @@
       <c r="F5" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="G5" s="1" t="s">
+      <c r="G5" s="14" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="9" t="s">
+      <c r="A6" s="16" t="s">
         <v>101</v>
       </c>
       <c r="B6" s="13" t="s">
@@ -1005,12 +1025,12 @@
       <c r="F6" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="G6" s="1" t="s">
+      <c r="G6" s="14" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="9" t="s">
+      <c r="A7" s="16" t="s">
         <v>102</v>
       </c>
       <c r="B7" s="13" t="s">
@@ -1022,7 +1042,7 @@
       <c r="E7" s="4"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="9" t="s">
+      <c r="A8" s="16" t="s">
         <v>103</v>
       </c>
       <c r="B8" s="13" t="s">
@@ -1034,7 +1054,7 @@
       <c r="E8" s="4"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="9" t="s">
+      <c r="A9" s="16" t="s">
         <v>104</v>
       </c>
       <c r="B9" s="13" t="s">
@@ -1046,7 +1066,7 @@
       <c r="E9" s="4"/>
     </row>
     <row r="10" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="9" t="s">
+      <c r="A10" s="16" t="s">
         <v>105</v>
       </c>
       <c r="B10" s="13" t="s">
@@ -1097,7 +1117,7 @@
       <c r="E14" s="5"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="9" t="s">
+      <c r="A15" s="16" t="s">
         <v>106</v>
       </c>
       <c r="B15" s="13" t="s">
@@ -1115,7 +1135,7 @@
       <c r="F15" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="G15" s="1" t="s">
+      <c r="G15" s="14" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1129,7 +1149,7 @@
       <c r="F16" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="G16" s="1" t="s">
+      <c r="G16" s="14" t="s">
         <v>19</v>
       </c>
     </row>
@@ -1143,7 +1163,7 @@
       <c r="F17" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="G17" s="1" t="s">
+      <c r="G17" s="14" t="s">
         <v>23</v>
       </c>
     </row>
@@ -1157,7 +1177,7 @@
       <c r="F18" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="G18" s="1" t="s">
+      <c r="G18" s="14" t="s">
         <v>24</v>
       </c>
     </row>
@@ -1171,7 +1191,7 @@
       <c r="F19" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="G19" s="1" t="s">
+      <c r="G19" s="14" t="s">
         <v>25</v>
       </c>
     </row>
@@ -1185,7 +1205,7 @@
       <c r="F20" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="G20" s="1" t="s">
+      <c r="G20" s="14" t="s">
         <v>26</v>
       </c>
     </row>
@@ -1199,7 +1219,7 @@
       <c r="F21" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="G21" s="1" t="s">
+      <c r="G21" s="14" t="s">
         <v>27</v>
       </c>
     </row>
@@ -1214,7 +1234,7 @@
       <c r="F22" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="G22" s="1" t="s">
+      <c r="G22" s="14" t="s">
         <v>28</v>
       </c>
     </row>
@@ -1237,7 +1257,7 @@
       <c r="F23" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="G23" s="1" t="s">
+      <c r="G23" s="14" t="s">
         <v>29</v>
       </c>
     </row>
@@ -1257,7 +1277,7 @@
       <c r="F24" s="13" t="s">
         <v>107</v>
       </c>
-      <c r="G24" s="1" t="s">
+      <c r="G24" s="14" t="s">
         <v>108</v>
       </c>
     </row>
@@ -1277,7 +1297,7 @@
       <c r="F25" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="G25" s="1" t="s">
+      <c r="G25" s="14" t="s">
         <v>30</v>
       </c>
     </row>
@@ -1297,12 +1317,12 @@
       <c r="F26" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="G26" s="1" t="s">
+      <c r="G26" s="14" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="9" t="s">
+      <c r="A27" s="15" t="s">
         <v>127</v>
       </c>
       <c r="B27" s="13" t="s">
@@ -1317,7 +1337,7 @@
       <c r="F27" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="G27" s="1" t="s">
+      <c r="G27" s="14" t="s">
         <v>32</v>
       </c>
     </row>
@@ -1354,7 +1374,7 @@
       <c r="F29" s="13" t="s">
         <v>109</v>
       </c>
-      <c r="G29" s="1" t="s">
+      <c r="G29" s="14" t="s">
         <v>111</v>
       </c>
     </row>
@@ -1375,7 +1395,7 @@
       <c r="F30" s="13" t="s">
         <v>110</v>
       </c>
-      <c r="G30" s="1" t="s">
+      <c r="G30" s="17" t="s">
         <v>112</v>
       </c>
     </row>

</xml_diff>